<commit_message>
regenerated DEseq results based on psuedo count split by genotype, sex, age, and replicate.
</commit_message>
<xml_diff>
--- a/GSE107451/processed_data/DESeq_result/DESeq_DGRP-551_female_50_vs_3_DOWN0.05.xlsx
+++ b/GSE107451/processed_data/DESeq_result/DESeq_DGRP-551_female_50_vs_3_DOWN0.05.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="107">
   <si>
     <t xml:space="preserve"/>
   </si>
@@ -38,7 +38,7 @@
     <t xml:space="preserve">sig</t>
   </si>
   <si>
-    <t xml:space="preserve">Hsp83</t>
+    <t xml:space="preserve">mt:lrRNA</t>
   </si>
   <si>
     <t xml:space="preserve">down</t>
@@ -47,148 +47,292 @@
     <t xml:space="preserve">Hsromega</t>
   </si>
   <si>
-    <t xml:space="preserve">Hsp26</t>
-  </si>
-  <si>
-    <t xml:space="preserve">mt:lrRNA</t>
+    <t xml:space="preserve">FMRFa</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CG14645</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CCAP</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CG11458</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TM4SF</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CG15213</t>
+  </si>
+  <si>
+    <t xml:space="preserve">mt:ND6</t>
+  </si>
+  <si>
+    <t xml:space="preserve">betaTry</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CG31997</t>
+  </si>
+  <si>
+    <t xml:space="preserve">alphaTry</t>
+  </si>
+  <si>
+    <t xml:space="preserve">mt:ND5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">mt:ND3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Thd1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CG7582</t>
+  </si>
+  <si>
+    <t xml:space="preserve">mt:ND2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">rad</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Dop2R</t>
+  </si>
+  <si>
+    <t xml:space="preserve">mt:ND4</t>
   </si>
   <si>
     <t xml:space="preserve">mt:CoIII</t>
   </si>
   <si>
-    <t xml:space="preserve">TM4SF</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Hsp23</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Atpalpha</t>
-  </si>
-  <si>
-    <t xml:space="preserve">mt:ND5</t>
-  </si>
-  <si>
-    <t xml:space="preserve">jim</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Hsp70Bc</t>
-  </si>
-  <si>
-    <t xml:space="preserve">pan</t>
-  </si>
-  <si>
-    <t xml:space="preserve">unc-13</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CaMKII</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Syt1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Cyt-c-p</t>
-  </si>
-  <si>
-    <t xml:space="preserve">DnaJ-1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">bun</t>
-  </si>
-  <si>
-    <t xml:space="preserve">sm</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Dop2R</t>
-  </si>
-  <si>
-    <t xml:space="preserve">nrv3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">qvr</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Vha16-1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">mei-P26</t>
-  </si>
-  <si>
-    <t xml:space="preserve">14-3-3zeta</t>
+    <t xml:space="preserve">Gad1</t>
   </si>
   <si>
     <t xml:space="preserve">Mpcp2</t>
   </si>
   <si>
-    <t xml:space="preserve">Hsp68</t>
-  </si>
-  <si>
-    <t xml:space="preserve">mt:ND6</t>
-  </si>
-  <si>
-    <t xml:space="preserve">para</t>
-  </si>
-  <si>
-    <t xml:space="preserve">levy</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Sh</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Rdl</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Vha13</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RNASEK</t>
-  </si>
-  <si>
-    <t xml:space="preserve">mt:ND4</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ATPsynF</t>
-  </si>
-  <si>
-    <t xml:space="preserve">porin</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CG6329</t>
-  </si>
-  <si>
-    <t xml:space="preserve">COX4</t>
-  </si>
-  <si>
     <t xml:space="preserve">jdp</t>
   </si>
   <si>
-    <t xml:space="preserve">COX6B</t>
-  </si>
-  <si>
-    <t xml:space="preserve">mub</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Ggamma30A</t>
-  </si>
-  <si>
-    <t xml:space="preserve">rad</t>
-  </si>
-  <si>
-    <t xml:space="preserve">bru3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">sesB</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Hsp27</t>
-  </si>
-  <si>
-    <t xml:space="preserve">pros</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Hsp67Bc</t>
-  </si>
-  <si>
-    <t xml:space="preserve">cpx</t>
+    <t xml:space="preserve">Cadps</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CG32432</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CG32000</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CG31077</t>
+  </si>
+  <si>
+    <t xml:space="preserve">hbn</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Nplp3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tob</t>
+  </si>
+  <si>
+    <t xml:space="preserve">prim</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CG7768</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Corin</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CR44024</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CG42402</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CG3906</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Nckx30C</t>
+  </si>
+  <si>
+    <t xml:space="preserve">AP-2mu</t>
+  </si>
+  <si>
+    <t xml:space="preserve">tapas</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CG13375</t>
+  </si>
+  <si>
+    <t xml:space="preserve">nAChRalpha4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Rab3-GEF</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fer1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Asator</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mf</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CG9636</t>
+  </si>
+  <si>
+    <t xml:space="preserve">mGluR</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CG4000</t>
+  </si>
+  <si>
+    <t xml:space="preserve">larp</t>
+  </si>
+  <si>
+    <t xml:space="preserve">dpr11</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CG42795</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Antp</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mhc</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sls</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CG11319</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CG4115</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RhoGEF3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Epac</t>
+  </si>
+  <si>
+    <t xml:space="preserve">onecut</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sun</t>
+  </si>
+  <si>
+    <t xml:space="preserve">tty</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Snmp2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Task6</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SPoCk</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CG43778</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CG42340</t>
+  </si>
+  <si>
+    <t xml:space="preserve">mt:srRNA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">drd</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Shal</t>
+  </si>
+  <si>
+    <t xml:space="preserve">eIF4G2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CG11099</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CG17698</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CG31211</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NetB</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CG43134</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CR45333</t>
+  </si>
+  <si>
+    <t xml:space="preserve">beat-Ib</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mlc2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CG4467</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cht8</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CG31998</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CG6749</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CG32444</t>
+  </si>
+  <si>
+    <t xml:space="preserve">fz</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CR44922</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mid1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tg</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cpr49Ae</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CG34371</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CG15515</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CG11294</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sfl</t>
+  </si>
+  <si>
+    <t xml:space="preserve">kis</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CG34330</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Vps11</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CG9990</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TrissinR</t>
   </si>
 </sst>
 </file>
@@ -551,22 +695,22 @@
         <v>8</v>
       </c>
       <c r="B2" t="n">
-        <v>5.50748476523922</v>
+        <v>20334.5502871809</v>
       </c>
       <c r="C2" t="n">
-        <v>-2.00496021504214</v>
+        <v>-2.70346666387554</v>
       </c>
       <c r="D2" t="n">
-        <v>0.0524397684983857</v>
+        <v>0.30313716655663</v>
       </c>
       <c r="E2" t="n">
-        <v>-38.2335824976775</v>
+        <v>-8.918294957311</v>
       </c>
       <c r="F2" t="n">
-        <v>0</v>
+        <v>0.000000000000000000473521863432367</v>
       </c>
       <c r="G2" t="n">
-        <v>0</v>
+        <v>0.000000000000000825348607962615</v>
       </c>
       <c r="H2" t="s">
         <v>9</v>
@@ -577,22 +721,22 @@
         <v>10</v>
       </c>
       <c r="B3" t="n">
-        <v>22.2400881132626</v>
+        <v>21401.2747626466</v>
       </c>
       <c r="C3" t="n">
-        <v>-2.63570659778479</v>
+        <v>-2.25148559305382</v>
       </c>
       <c r="D3" t="n">
-        <v>0.0489611227092166</v>
+        <v>0.291438341626582</v>
       </c>
       <c r="E3" t="n">
-        <v>-53.8326421442258</v>
+        <v>-7.7254268621204</v>
       </c>
       <c r="F3" t="n">
-        <v>0</v>
+        <v>0.0000000000000111479134141038</v>
       </c>
       <c r="G3" t="n">
-        <v>0</v>
+        <v>0.0000000000129538753871886</v>
       </c>
       <c r="H3" t="s">
         <v>9</v>
@@ -603,22 +747,22 @@
         <v>11</v>
       </c>
       <c r="B4" t="n">
-        <v>5.50190585266755</v>
+        <v>236.522069236308</v>
       </c>
       <c r="C4" t="n">
-        <v>-2.76204309176084</v>
+        <v>-8.88162299099374</v>
       </c>
       <c r="D4" t="n">
-        <v>0.0699000618336067</v>
+        <v>1.58119636331201</v>
       </c>
       <c r="E4" t="n">
-        <v>-39.5141723670536</v>
+        <v>-5.61702720615299</v>
       </c>
       <c r="F4" t="n">
-        <v>0</v>
+        <v>0.0000000194270843538782</v>
       </c>
       <c r="G4" t="n">
-        <v>0</v>
+        <v>0.00000752475733973547</v>
       </c>
       <c r="H4" t="s">
         <v>9</v>
@@ -629,22 +773,22 @@
         <v>12</v>
       </c>
       <c r="B5" t="n">
-        <v>21.3447993631862</v>
+        <v>160.694624390936</v>
       </c>
       <c r="C5" t="n">
-        <v>-3.02945297673246</v>
+        <v>-6.73384654851594</v>
       </c>
       <c r="D5" t="n">
-        <v>0.042539025047058</v>
+        <v>1.52961016840446</v>
       </c>
       <c r="E5" t="n">
-        <v>-71.2158535222937</v>
+        <v>-4.4023285720832</v>
       </c>
       <c r="F5" t="n">
-        <v>0</v>
+        <v>0.0000107095202825485</v>
       </c>
       <c r="G5" t="n">
-        <v>0</v>
+        <v>0.00160957625823787</v>
       </c>
       <c r="H5" t="s">
         <v>9</v>
@@ -655,22 +799,22 @@
         <v>13</v>
       </c>
       <c r="B6" t="n">
-        <v>9.81712020096401</v>
+        <v>351.690206362731</v>
       </c>
       <c r="C6" t="n">
-        <v>-1.43669051998797</v>
+        <v>-24.2520989444166</v>
       </c>
       <c r="D6" t="n">
-        <v>0.0418170409049414</v>
+        <v>5.94835645642157</v>
       </c>
       <c r="E6" t="n">
-        <v>-34.3565802098207</v>
+        <v>-4.07710921867083</v>
       </c>
       <c r="F6" t="n">
-        <v>1.12324499951912e-258</v>
+        <v>0.0000455990769822145</v>
       </c>
       <c r="G6" t="n">
-        <v>1.24174734696838e-255</v>
+        <v>0.0057803048130909</v>
       </c>
       <c r="H6" t="s">
         <v>9</v>
@@ -681,22 +825,22 @@
         <v>14</v>
       </c>
       <c r="B7" t="n">
-        <v>2.88698351845481</v>
+        <v>320.125878813587</v>
       </c>
       <c r="C7" t="n">
-        <v>-1.33971308133355</v>
+        <v>-24.118357795</v>
       </c>
       <c r="D7" t="n">
-        <v>0.0399113539368419</v>
+        <v>5.94837631674885</v>
       </c>
       <c r="E7" t="n">
-        <v>-33.5672170744593</v>
+        <v>-4.05461196647729</v>
       </c>
       <c r="F7" t="n">
-        <v>5.04935294405752e-247</v>
+        <v>0.0000502175929109211</v>
       </c>
       <c r="G7" t="n">
-        <v>4.78462258256193e-244</v>
+        <v>0.00614240452236741</v>
       </c>
       <c r="H7" t="s">
         <v>9</v>
@@ -707,22 +851,22 @@
         <v>15</v>
       </c>
       <c r="B8" t="n">
-        <v>3.89043674548176</v>
+        <v>1779.10498416831</v>
       </c>
       <c r="C8" t="n">
-        <v>-2.30776476806951</v>
+        <v>-1.59457450211636</v>
       </c>
       <c r="D8" t="n">
-        <v>0.0692773135912738</v>
+        <v>0.398127231718256</v>
       </c>
       <c r="E8" t="n">
-        <v>-33.3119840888316</v>
+        <v>-4.00518822898504</v>
       </c>
       <c r="F8" t="n">
-        <v>2.58940450931383e-243</v>
+        <v>0.0000619681165399778</v>
       </c>
       <c r="G8" t="n">
-        <v>2.14694001378483e-240</v>
+        <v>0.0071616754765918</v>
       </c>
       <c r="H8" t="s">
         <v>9</v>
@@ -733,22 +877,22 @@
         <v>16</v>
       </c>
       <c r="B9" t="n">
-        <v>10.3882778717397</v>
+        <v>213.770008331718</v>
       </c>
       <c r="C9" t="n">
-        <v>-1.26303188352423</v>
+        <v>-23.5567234326622</v>
       </c>
       <c r="D9" t="n">
-        <v>0.0405141231360315</v>
+        <v>5.94848622498377</v>
       </c>
       <c r="E9" t="n">
-        <v>-31.1751010699019</v>
+        <v>-3.96012069990571</v>
       </c>
       <c r="F9" t="n">
-        <v>2.31804479439009e-213</v>
+        <v>0.0000749118906155431</v>
       </c>
       <c r="G9" t="n">
-        <v>1.7083990134655e-210</v>
+        <v>0.00816071408393073</v>
       </c>
       <c r="H9" t="s">
         <v>9</v>
@@ -759,22 +903,22 @@
         <v>17</v>
       </c>
       <c r="B10" t="n">
-        <v>3.63287051427373</v>
+        <v>1248.09082576037</v>
       </c>
       <c r="C10" t="n">
-        <v>-1.24645887915222</v>
+        <v>-1.44418943537042</v>
       </c>
       <c r="D10" t="n">
-        <v>0.0412469761579248</v>
+        <v>0.369863851830386</v>
       </c>
       <c r="E10" t="n">
-        <v>-30.2194001902062</v>
+        <v>-3.9046514770865</v>
       </c>
       <c r="F10" t="n">
-        <v>0.0000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000131729073722348</v>
+        <v>0.0000943612737708621</v>
       </c>
       <c r="G10" t="n">
-        <v>0.00000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000873758946000332</v>
+        <v>0.0101213353958531</v>
       </c>
       <c r="H10" t="s">
         <v>9</v>
@@ -785,22 +929,22 @@
         <v>18</v>
       </c>
       <c r="B11" t="n">
-        <v>9.19964933624738</v>
+        <v>129.637752577403</v>
       </c>
       <c r="C11" t="n">
-        <v>-1.2864589618061</v>
+        <v>-22.8964777781204</v>
       </c>
       <c r="D11" t="n">
-        <v>0.0436211946124172</v>
+        <v>5.94870099447364</v>
       </c>
       <c r="E11" t="n">
-        <v>-29.4916031813557</v>
+        <v>-3.84898783774664</v>
       </c>
       <c r="F11" t="n">
-        <v>0.0000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000368909163264726</v>
+        <v>0.000118606895492403</v>
       </c>
       <c r="G11" t="n">
-        <v>0.000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000022245222544863</v>
+        <v>0.0119844532662759</v>
       </c>
       <c r="H11" t="s">
         <v>9</v>
@@ -811,22 +955,22 @@
         <v>19</v>
       </c>
       <c r="B12" t="n">
-        <v>2.67409403196711</v>
+        <v>227.086039179675</v>
       </c>
       <c r="C12" t="n">
-        <v>-1.71670625918585</v>
+        <v>-2.00725471837067</v>
       </c>
       <c r="D12" t="n">
-        <v>0.0583523583594368</v>
+        <v>0.525105070890182</v>
       </c>
       <c r="E12" t="n">
-        <v>-29.4196551339253</v>
+        <v>-3.82257728908974</v>
       </c>
       <c r="F12" t="n">
-        <v>0.000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000307869917541631</v>
+        <v>0.000132064064750592</v>
       </c>
       <c r="G12" t="n">
-        <v>0.000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000170175096921136</v>
+        <v>0.0127300403272057</v>
       </c>
       <c r="H12" t="s">
         <v>9</v>
@@ -837,22 +981,22 @@
         <v>20</v>
       </c>
       <c r="B13" t="n">
-        <v>3.74032549928798</v>
+        <v>106.355870481869</v>
       </c>
       <c r="C13" t="n">
-        <v>-1.01617596269551</v>
+        <v>-22.5122489564538</v>
       </c>
       <c r="D13" t="n">
-        <v>0.0345989296795211</v>
+        <v>5.94882040613114</v>
       </c>
       <c r="E13" t="n">
-        <v>-29.3701560166174</v>
+        <v>-3.78432149897342</v>
       </c>
       <c r="F13" t="n">
-        <v>0.00000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000132131044926368</v>
+        <v>0.00015412848062778</v>
       </c>
       <c r="G13" t="n">
-        <v>0.00000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000067417324692046</v>
+        <v>0.0137767149607293</v>
       </c>
       <c r="H13" t="s">
         <v>9</v>
@@ -863,22 +1007,22 @@
         <v>21</v>
       </c>
       <c r="B14" t="n">
-        <v>5.92145039871603</v>
+        <v>2528.99039610526</v>
       </c>
       <c r="C14" t="n">
-        <v>-1.11677206929169</v>
+        <v>-1.2015264823517</v>
       </c>
       <c r="D14" t="n">
-        <v>0.0385108283008942</v>
+        <v>0.317893416194152</v>
       </c>
       <c r="E14" t="n">
-        <v>-28.9989106587396</v>
+        <v>-3.77965198756389</v>
       </c>
       <c r="F14" t="n">
-        <v>0.0000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000679099352956681</v>
+        <v>0.000157047706860855</v>
       </c>
       <c r="G14" t="n">
-        <v>0.0000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000321747572011547</v>
+        <v>0.0138599571168846</v>
       </c>
       <c r="H14" t="s">
         <v>9</v>
@@ -889,22 +1033,22 @@
         <v>22</v>
       </c>
       <c r="B15" t="n">
-        <v>3.67513243937436</v>
+        <v>440.985973382831</v>
       </c>
       <c r="C15" t="n">
-        <v>-1.09874230042491</v>
+        <v>-1.89373234920345</v>
       </c>
       <c r="D15" t="n">
-        <v>0.0388426725545552</v>
+        <v>0.515546093331108</v>
       </c>
       <c r="E15" t="n">
-        <v>-28.2869902651962</v>
+        <v>-3.6732551632143</v>
       </c>
       <c r="F15" t="n">
-        <v>0.0000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000499595214137418</v>
+        <v>0.000239480131640896</v>
       </c>
       <c r="G15" t="n">
-        <v>0.0000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000207113440960843</v>
+        <v>0.0181484291065253</v>
       </c>
       <c r="H15" t="s">
         <v>9</v>
@@ -915,22 +1059,22 @@
         <v>23</v>
       </c>
       <c r="B16" t="n">
-        <v>5.10170641828465</v>
+        <v>836.017991262992</v>
       </c>
       <c r="C16" t="n">
-        <v>-1.14773925493967</v>
+        <v>-1.31592005470418</v>
       </c>
       <c r="D16" t="n">
-        <v>0.0425607073611776</v>
+        <v>0.366408042415366</v>
       </c>
       <c r="E16" t="n">
-        <v>-26.9671094796372</v>
+        <v>-3.59140603473008</v>
       </c>
       <c r="F16" t="n">
-        <v>0.000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000359426073199254</v>
+        <v>0.000328898760557927</v>
       </c>
       <c r="G16" t="n">
-        <v>0.000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000132448507973925</v>
+        <v>0.0224811976334301</v>
       </c>
       <c r="H16" t="s">
         <v>9</v>
@@ -941,22 +1085,22 @@
         <v>24</v>
       </c>
       <c r="B17" t="n">
-        <v>4.67677440989091</v>
+        <v>498.338575327873</v>
       </c>
       <c r="C17" t="n">
-        <v>-1.22797882825045</v>
+        <v>-1.47930609834793</v>
       </c>
       <c r="D17" t="n">
-        <v>0.0457809723090687</v>
+        <v>0.419948151811819</v>
       </c>
       <c r="E17" t="n">
-        <v>-26.8229084336681</v>
+        <v>-3.52259223422136</v>
       </c>
       <c r="F17" t="n">
-        <v>0.0000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000174683134558196</v>
+        <v>0.000427348312172383</v>
       </c>
       <c r="G17" t="n">
-        <v>0.00000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000609828016591848</v>
+        <v>0.0275877077080172</v>
       </c>
       <c r="H17" t="s">
         <v>9</v>
@@ -967,22 +1111,22 @@
         <v>25</v>
       </c>
       <c r="B18" t="n">
-        <v>2.12234455824168</v>
+        <v>232.689272937672</v>
       </c>
       <c r="C18" t="n">
-        <v>-1.32221623180551</v>
+        <v>-1.81844362869608</v>
       </c>
       <c r="D18" t="n">
-        <v>0.0496982680019245</v>
+        <v>0.520641053043384</v>
       </c>
       <c r="E18" t="n">
-        <v>-26.6048754808581</v>
+        <v>-3.49270119608596</v>
       </c>
       <c r="F18" t="n">
-        <v>0.00000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000596125575745143</v>
+        <v>0.00047816123205219</v>
       </c>
       <c r="G18" t="n">
-        <v>0.00000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000197705047195877</v>
+        <v>0.0305847716501639</v>
       </c>
       <c r="H18" t="s">
         <v>9</v>
@@ -993,22 +1137,22 @@
         <v>26</v>
       </c>
       <c r="B19" t="n">
-        <v>4.46155374778474</v>
+        <v>1725.76892787567</v>
       </c>
       <c r="C19" t="n">
-        <v>-1.02750947870658</v>
+        <v>-1.14454354566748</v>
       </c>
       <c r="D19" t="n">
-        <v>0.0388986391710851</v>
+        <v>0.329516784588943</v>
       </c>
       <c r="E19" t="n">
-        <v>-26.4150494876532</v>
+        <v>-3.47339983635507</v>
       </c>
       <c r="F19" t="n">
-        <v>0.00000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000092030161951973</v>
+        <v>0.000513909142041306</v>
       </c>
       <c r="G19" t="n">
-        <v>0.000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000290683840108303</v>
+        <v>0.0322790498947026</v>
       </c>
       <c r="H19" t="s">
         <v>9</v>
@@ -1019,22 +1163,22 @@
         <v>27</v>
       </c>
       <c r="B20" t="n">
-        <v>4.72230017198741</v>
+        <v>10456.3583805902</v>
       </c>
       <c r="C20" t="n">
-        <v>-1.18975230954096</v>
+        <v>-1.25702122394205</v>
       </c>
       <c r="D20" t="n">
-        <v>0.0456606185441673</v>
+        <v>0.364177855096033</v>
       </c>
       <c r="E20" t="n">
-        <v>-26.0564212109855</v>
+        <v>-3.45166848107932</v>
       </c>
       <c r="F20" t="n">
-        <v>0.0000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000113781823741185</v>
+        <v>0.000557131802605298</v>
       </c>
       <c r="G20" t="n">
-        <v>0.00000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000343052198579672</v>
+        <v>0.0343745391837534</v>
       </c>
       <c r="H20" t="s">
         <v>9</v>
@@ -1045,22 +1189,22 @@
         <v>28</v>
       </c>
       <c r="B21" t="n">
-        <v>12.1631056241584</v>
+        <v>1665.87149422986</v>
       </c>
       <c r="C21" t="n">
-        <v>-1.7265109343153</v>
+        <v>-1.15491560184898</v>
       </c>
       <c r="D21" t="n">
-        <v>0.066958740525792</v>
+        <v>0.341330562954855</v>
       </c>
       <c r="E21" t="n">
-        <v>-25.7846984689065</v>
+        <v>-3.38356926450131</v>
       </c>
       <c r="F21" t="n">
-        <v>0.0000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000131655034660907</v>
+        <v>0.000715501572755824</v>
       </c>
       <c r="G21" t="n">
-        <v>0.00000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000349307137962317</v>
+        <v>0.0408891554528984</v>
       </c>
       <c r="H21" t="s">
         <v>9</v>
@@ -1071,22 +1215,22 @@
         <v>29</v>
       </c>
       <c r="B22" t="n">
-        <v>14.1652755360089</v>
+        <v>8385.32039462827</v>
       </c>
       <c r="C22" t="n">
-        <v>-1.29622200041438</v>
+        <v>-1.01189006689574</v>
       </c>
       <c r="D22" t="n">
-        <v>0.0503727290483613</v>
+        <v>0.300800759505146</v>
       </c>
       <c r="E22" t="n">
-        <v>-25.7326141525888</v>
+        <v>-3.36398773912811</v>
       </c>
       <c r="F22" t="n">
-        <v>0.000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000050462879245798</v>
+        <v>0.000768249561351883</v>
       </c>
       <c r="G22" t="n">
-        <v>0.0000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000128738568475915</v>
+        <v>0.0428498875339627</v>
       </c>
       <c r="H22" t="s">
         <v>9</v>
@@ -1097,22 +1241,22 @@
         <v>30</v>
       </c>
       <c r="B23" t="n">
-        <v>4.14266723834142</v>
+        <v>1020.69582443088</v>
       </c>
       <c r="C23" t="n">
-        <v>-1.01332206505518</v>
+        <v>-1.1986590393874</v>
       </c>
       <c r="D23" t="n">
-        <v>0.0395980045217306</v>
+        <v>0.357401642010582</v>
       </c>
       <c r="E23" t="n">
-        <v>-25.5902305506099</v>
+        <v>-3.35381514378132</v>
       </c>
       <c r="F23" t="n">
-        <v>0.00000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000195967825530893</v>
+        <v>0.000797055921091972</v>
       </c>
       <c r="G23" t="n">
-        <v>0.000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000481427624720893</v>
+        <v>0.0441037609670891</v>
       </c>
       <c r="H23" t="s">
         <v>9</v>
@@ -1123,22 +1267,22 @@
         <v>31</v>
       </c>
       <c r="B24" t="n">
-        <v>6.21324231063165</v>
+        <v>1999.13653830667</v>
       </c>
       <c r="C24" t="n">
-        <v>-1.05577862440852</v>
+        <v>-1.04991085159922</v>
       </c>
       <c r="D24" t="n">
-        <v>0.0414965311712782</v>
+        <v>0.323062329239544</v>
       </c>
       <c r="E24" t="n">
-        <v>-25.4425754299982</v>
+        <v>-3.2498708656952</v>
       </c>
       <c r="F24" t="n">
-        <v>0.0000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000853002099156996</v>
+        <v>0.00115457423418218</v>
       </c>
       <c r="G24" t="n">
-        <v>0.0000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000202070104418155</v>
+        <v>0.0591889085346923</v>
       </c>
       <c r="H24" t="s">
         <v>9</v>
@@ -1149,22 +1293,22 @@
         <v>32</v>
       </c>
       <c r="B25" t="n">
-        <v>6.87046616495375</v>
+        <v>4183.06843366928</v>
       </c>
       <c r="C25" t="n">
-        <v>-1.00104040334324</v>
+        <v>-1.02642702220787</v>
       </c>
       <c r="D25" t="n">
-        <v>0.0394011547641826</v>
+        <v>0.316491657308568</v>
       </c>
       <c r="E25" t="n">
-        <v>-25.4063722074774</v>
+        <v>-3.24314084907187</v>
       </c>
       <c r="F25" t="n">
-        <v>0.000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000214443087838146</v>
+        <v>0.00118219752818961</v>
       </c>
       <c r="G25" t="n">
-        <v>0.000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000049048310401049</v>
+        <v>0.0595615831019127</v>
       </c>
       <c r="H25" t="s">
         <v>9</v>
@@ -1175,22 +1319,22 @@
         <v>33</v>
       </c>
       <c r="B26" t="n">
-        <v>10.1987661741933</v>
+        <v>1286.48556329442</v>
       </c>
       <c r="C26" t="n">
-        <v>-1.08773310045093</v>
+        <v>-1.07670033120351</v>
       </c>
       <c r="D26" t="n">
-        <v>0.0429494597054976</v>
+        <v>0.34003367470006</v>
       </c>
       <c r="E26" t="n">
-        <v>-25.3258855387113</v>
+        <v>-3.16645206435291</v>
       </c>
       <c r="F26" t="n">
-        <v>0.00000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000165713055512437</v>
+        <v>0.00154310776677933</v>
       </c>
       <c r="G26" t="n">
-        <v>0.000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000366391565737999</v>
+        <v>0.0755554141747116</v>
       </c>
       <c r="H26" t="s">
         <v>9</v>
@@ -1201,22 +1345,22 @@
         <v>34</v>
       </c>
       <c r="B27" t="n">
-        <v>3.09149301778399</v>
+        <v>373.230038787951</v>
       </c>
       <c r="C27" t="n">
-        <v>-1.06827848882395</v>
+        <v>-1.45916749285706</v>
       </c>
       <c r="D27" t="n">
-        <v>0.0421901848330566</v>
+        <v>0.474282135747765</v>
       </c>
       <c r="E27" t="n">
-        <v>-25.3205453602786</v>
+        <v>-3.07658118001113</v>
       </c>
       <c r="F27" t="n">
-        <v>0.00000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000189748294574459</v>
+        <v>0.00209389277420608</v>
       </c>
       <c r="G27" t="n">
-        <v>0.000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000406000141262061</v>
+        <v>0.0941846478823535</v>
       </c>
       <c r="H27" t="s">
         <v>9</v>
@@ -1227,22 +1371,22 @@
         <v>35</v>
       </c>
       <c r="B28" t="n">
-        <v>2.14016711511802</v>
+        <v>1030.43634062309</v>
       </c>
       <c r="C28" t="n">
-        <v>-1.48632456230847</v>
+        <v>-1.39021529304345</v>
       </c>
       <c r="D28" t="n">
-        <v>0.0587649788495795</v>
+        <v>0.455797582696365</v>
       </c>
       <c r="E28" t="n">
-        <v>-25.2926928828309</v>
+        <v>-3.05007166738214</v>
       </c>
       <c r="F28" t="n">
-        <v>0.00000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000384386154078271</v>
+        <v>0.00228786765037083</v>
       </c>
       <c r="G28" t="n">
-        <v>0.000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000796760425000366</v>
+        <v>0.101598810562964</v>
       </c>
       <c r="H28" t="s">
         <v>9</v>
@@ -1253,22 +1397,22 @@
         <v>36</v>
       </c>
       <c r="B29" t="n">
-        <v>2.30973821859066</v>
+        <v>28.9628102843333</v>
       </c>
       <c r="C29" t="n">
-        <v>-1.07348258351066</v>
+        <v>-8.30156415545547</v>
       </c>
       <c r="D29" t="n">
-        <v>0.0424991606161929</v>
+        <v>2.81516789573403</v>
       </c>
       <c r="E29" t="n">
-        <v>-25.2589125984207</v>
+        <v>-2.9488700009812</v>
       </c>
       <c r="F29" t="n">
-        <v>0.00000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000903976873967242</v>
+        <v>0.00318938104373623</v>
       </c>
       <c r="G29" t="n">
-        <v>0.00000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000181699351667416</v>
+        <v>0.12953934985332</v>
       </c>
       <c r="H29" t="s">
         <v>9</v>
@@ -1279,22 +1423,22 @@
         <v>37</v>
       </c>
       <c r="B30" t="n">
-        <v>4.30207453661182</v>
+        <v>119.407722483004</v>
       </c>
       <c r="C30" t="n">
-        <v>-1.096263563398</v>
+        <v>-2.05386817012563</v>
       </c>
       <c r="D30" t="n">
-        <v>0.0435435261178827</v>
+        <v>0.702283409470277</v>
       </c>
       <c r="E30" t="n">
-        <v>-25.176269841587</v>
+        <v>-2.92455743995837</v>
       </c>
       <c r="F30" t="n">
-        <v>0.0000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000728900261595383</v>
+        <v>0.00344946411549065</v>
       </c>
       <c r="G30" t="n">
-        <v>0.0000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000142199865740064</v>
+        <v>0.135873806854242</v>
       </c>
       <c r="H30" t="s">
         <v>9</v>
@@ -1305,22 +1449,22 @@
         <v>38</v>
       </c>
       <c r="B31" t="n">
-        <v>4.50929999102243</v>
+        <v>15.4792098442681</v>
       </c>
       <c r="C31" t="n">
-        <v>-1.1337889007415</v>
+        <v>-7.3880957198738</v>
       </c>
       <c r="D31" t="n">
-        <v>0.0450659125860809</v>
+        <v>2.63155360439423</v>
       </c>
       <c r="E31" t="n">
-        <v>-25.1584587037006</v>
+        <v>-2.8075034107369</v>
       </c>
       <c r="F31" t="n">
-        <v>0.000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000114196049079032</v>
+        <v>0.00499271511405755</v>
       </c>
       <c r="G31" t="n">
-        <v>0.0000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000216417826726063</v>
+        <v>0.185330388212133</v>
       </c>
       <c r="H31" t="s">
         <v>9</v>
@@ -1331,22 +1475,22 @@
         <v>39</v>
       </c>
       <c r="B32" t="n">
-        <v>6.45820493035336</v>
+        <v>1450.53609982772</v>
       </c>
       <c r="C32" t="n">
-        <v>-1.02825942739651</v>
+        <v>-1.01873527891086</v>
       </c>
       <c r="D32" t="n">
-        <v>0.0410650382735795</v>
+        <v>0.363690511587143</v>
       </c>
       <c r="E32" t="n">
-        <v>-25.0397776460389</v>
+        <v>-2.80110491325471</v>
       </c>
       <c r="F32" t="n">
-        <v>0.0000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000022561615094084</v>
+        <v>0.0050927959194342</v>
       </c>
       <c r="G32" t="n">
-        <v>0.000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000404462683565024</v>
+        <v>0.186878806054185</v>
       </c>
       <c r="H32" t="s">
         <v>9</v>
@@ -1357,22 +1501,22 @@
         <v>40</v>
       </c>
       <c r="B33" t="n">
-        <v>6.15462976715739</v>
+        <v>485.364669772808</v>
       </c>
       <c r="C33" t="n">
-        <v>-1.08104435339478</v>
+        <v>-1.368710872426</v>
       </c>
       <c r="D33" t="n">
-        <v>0.0431879535313501</v>
+        <v>0.489662759495773</v>
       </c>
       <c r="E33" t="n">
-        <v>-25.0311548707685</v>
+        <v>-2.79521128753066</v>
       </c>
       <c r="F33" t="n">
-        <v>0.00000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000280073939928216</v>
+        <v>0.00518658053360464</v>
       </c>
       <c r="G33" t="n">
-        <v>0.000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000488876432511541</v>
+        <v>0.188337705626519</v>
       </c>
       <c r="H33" t="s">
         <v>9</v>
@@ -1383,22 +1527,22 @@
         <v>41</v>
       </c>
       <c r="B34" t="n">
-        <v>4.73977700026477</v>
+        <v>58.2368064866796</v>
       </c>
       <c r="C34" t="n">
-        <v>-1.03815122617529</v>
+        <v>-5.83964889558426</v>
       </c>
       <c r="D34" t="n">
-        <v>0.0415966188791927</v>
+        <v>2.10251961353937</v>
       </c>
       <c r="E34" t="n">
-        <v>-24.957586797868</v>
+        <v>-2.77745275619752</v>
       </c>
       <c r="F34" t="n">
-        <v>0.0000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000176653516701489</v>
+        <v>0.00547868040525795</v>
       </c>
       <c r="G34" t="n">
-        <v>0.00000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000300446865713072</v>
+        <v>0.194884488701319</v>
       </c>
       <c r="H34" t="s">
         <v>9</v>
@@ -1409,22 +1553,22 @@
         <v>42</v>
       </c>
       <c r="B35" t="n">
-        <v>5.29365227934646</v>
+        <v>799.491347295313</v>
       </c>
       <c r="C35" t="n">
-        <v>-1.06216446286787</v>
+        <v>-1.04904123211156</v>
       </c>
       <c r="D35" t="n">
-        <v>0.0427597579821572</v>
+        <v>0.378828956227712</v>
       </c>
       <c r="E35" t="n">
-        <v>-24.8402823821195</v>
+        <v>-2.76916855183844</v>
       </c>
       <c r="F35" t="n">
-        <v>0.00000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000032932869224952</v>
+        <v>0.00561995531128737</v>
       </c>
       <c r="G35" t="n">
-        <v>0.0000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000546109303922767</v>
+        <v>0.198399205621277</v>
       </c>
       <c r="H35" t="s">
         <v>9</v>
@@ -1435,22 +1579,22 @@
         <v>43</v>
       </c>
       <c r="B36" t="n">
-        <v>2.74993893182899</v>
+        <v>394.261775295132</v>
       </c>
       <c r="C36" t="n">
-        <v>-1.06408322804974</v>
+        <v>-1.21790104270758</v>
       </c>
       <c r="D36" t="n">
-        <v>0.0430612187942978</v>
+        <v>0.442911782289617</v>
       </c>
       <c r="E36" t="n">
-        <v>-24.7109407918257</v>
+        <v>-2.74975986507218</v>
       </c>
       <c r="F36" t="n">
-        <v>0.00000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000815818485740295</v>
+        <v>0.00596389527637486</v>
       </c>
       <c r="G36" t="n">
-        <v>0.00000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000128841047997985</v>
+        <v>0.204255784577384</v>
       </c>
       <c r="H36" t="s">
         <v>9</v>
@@ -1461,22 +1605,22 @@
         <v>44</v>
       </c>
       <c r="B37" t="n">
-        <v>4.78730555922371</v>
+        <v>595.975742856045</v>
       </c>
       <c r="C37" t="n">
-        <v>-1.06350643757195</v>
+        <v>-1.27466305085618</v>
       </c>
       <c r="D37" t="n">
-        <v>0.0434652251141873</v>
+        <v>0.464211264489454</v>
       </c>
       <c r="E37" t="n">
-        <v>-24.4679841132312</v>
+        <v>-2.74586841889344</v>
       </c>
       <c r="F37" t="n">
-        <v>0.00000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000323907803078137</v>
+        <v>0.00603509633146029</v>
       </c>
       <c r="G37" t="n">
-        <v>0.000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000477440101737173</v>
+        <v>0.204255784577384</v>
       </c>
       <c r="H37" t="s">
         <v>9</v>
@@ -1487,22 +1631,22 @@
         <v>45</v>
       </c>
       <c r="B38" t="n">
-        <v>4.12465744495796</v>
+        <v>154.061849606379</v>
       </c>
       <c r="C38" t="n">
-        <v>-1.06815524839568</v>
+        <v>-10.70428452385</v>
       </c>
       <c r="D38" t="n">
-        <v>0.0445739831269634</v>
+        <v>3.945545228163</v>
       </c>
       <c r="E38" t="n">
-        <v>-23.9636481521783</v>
+        <v>-2.71300515007245</v>
       </c>
       <c r="F38" t="n">
-        <v>0.000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000665938534343339</v>
+        <v>0.00666760703172154</v>
       </c>
       <c r="G38" t="n">
-        <v>0.0000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000920243812145702</v>
+        <v>0.217226898248423</v>
       </c>
       <c r="H38" t="s">
         <v>9</v>
@@ -1513,22 +1657,22 @@
         <v>46</v>
       </c>
       <c r="B39" t="n">
-        <v>4.66175649915569</v>
+        <v>1828.68826242787</v>
       </c>
       <c r="C39" t="n">
-        <v>-1.07492818340334</v>
+        <v>-1.02254022120339</v>
       </c>
       <c r="D39" t="n">
-        <v>0.0452335752641737</v>
+        <v>0.377812267287145</v>
       </c>
       <c r="E39" t="n">
-        <v>-23.7639447495701</v>
+        <v>-2.70647702507299</v>
       </c>
       <c r="F39" t="n">
-        <v>0.0000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000788433385334868</v>
+        <v>0.00680012875400493</v>
       </c>
       <c r="G39" t="n">
-        <v>0.0000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000106728135610738</v>
+        <v>0.220513942664755</v>
       </c>
       <c r="H39" t="s">
         <v>9</v>
@@ -1539,22 +1683,22 @@
         <v>47</v>
       </c>
       <c r="B40" t="n">
-        <v>4.61769111780656</v>
+        <v>113.662309020867</v>
       </c>
       <c r="C40" t="n">
-        <v>-1.04339608976926</v>
+        <v>-1.91098671844699</v>
       </c>
       <c r="D40" t="n">
-        <v>0.0447800444185967</v>
+        <v>0.71638916884908</v>
       </c>
       <c r="E40" t="n">
-        <v>-23.3004701830075</v>
+        <v>-2.66752597825717</v>
       </c>
       <c r="F40" t="n">
-        <v>0.00000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000438485859686537</v>
+        <v>0.00764119815465903</v>
       </c>
       <c r="G40" t="n">
-        <v>0.00000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000058169534146016</v>
+        <v>0.2432622535812</v>
       </c>
       <c r="H40" t="s">
         <v>9</v>
@@ -1565,22 +1709,22 @@
         <v>48</v>
       </c>
       <c r="B41" t="n">
-        <v>5.4157974003832</v>
+        <v>350.538855503041</v>
       </c>
       <c r="C41" t="n">
-        <v>-1.30501748661582</v>
+        <v>-1.19747420372479</v>
       </c>
       <c r="D41" t="n">
-        <v>0.0573118982068117</v>
+        <v>0.451476000387521</v>
       </c>
       <c r="E41" t="n">
-        <v>-22.7704460582796</v>
+        <v>-2.65235406244616</v>
       </c>
       <c r="F41" t="n">
-        <v>0.000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000900252030554991</v>
+        <v>0.007993267377698</v>
       </c>
       <c r="G41" t="n">
-        <v>0.000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000108570394884932</v>
+        <v>0.250633568318385</v>
       </c>
       <c r="H41" t="s">
         <v>9</v>
@@ -1591,22 +1735,22 @@
         <v>49</v>
       </c>
       <c r="B42" t="n">
-        <v>4.83587174990765</v>
+        <v>187.045433767188</v>
       </c>
       <c r="C42" t="n">
-        <v>-1.00351396623433</v>
+        <v>-1.46854642992108</v>
       </c>
       <c r="D42" t="n">
-        <v>0.0447482748102368</v>
+        <v>0.553881578998014</v>
       </c>
       <c r="E42" t="n">
-        <v>-22.4257576518852</v>
+        <v>-2.65137257783103</v>
       </c>
       <c r="F42" t="n">
-        <v>0.00000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000220706157206666</v>
+        <v>0.00801653553284565</v>
       </c>
       <c r="G42" t="n">
-        <v>0.000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000243990656791969</v>
+        <v>0.250633568318385</v>
       </c>
       <c r="H42" t="s">
         <v>9</v>
@@ -1617,22 +1761,22 @@
         <v>50</v>
       </c>
       <c r="B43" t="n">
-        <v>2.95807444512367</v>
+        <v>438.032852537035</v>
       </c>
       <c r="C43" t="n">
-        <v>-1.02338036708575</v>
+        <v>-1.11554275629782</v>
       </c>
       <c r="D43" t="n">
-        <v>0.0464084538422177</v>
+        <v>0.424391058857635</v>
       </c>
       <c r="E43" t="n">
-        <v>-22.0515936722457</v>
+        <v>-2.62857271145299</v>
       </c>
       <c r="F43" t="n">
-        <v>0.00000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000922185380738746</v>
+        <v>0.00857440226876795</v>
       </c>
       <c r="G43" t="n">
-        <v>0.00000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000089953759271178</v>
+        <v>0.262196195692325</v>
       </c>
       <c r="H43" t="s">
         <v>9</v>
@@ -1643,22 +1787,22 @@
         <v>51</v>
       </c>
       <c r="B44" t="n">
-        <v>8.586602018437</v>
+        <v>285.389956393055</v>
       </c>
       <c r="C44" t="n">
-        <v>-1.15208832253002</v>
+        <v>-1.38829572225754</v>
       </c>
       <c r="D44" t="n">
-        <v>0.0534564484878003</v>
+        <v>0.530927251190497</v>
       </c>
       <c r="E44" t="n">
-        <v>-21.5519054318199</v>
+        <v>-2.61485112912281</v>
       </c>
       <c r="F44" t="n">
-        <v>0.000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000508123156185922</v>
+        <v>0.00892663539677355</v>
       </c>
       <c r="G44" t="n">
-        <v>0.0000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000432100114741182</v>
+        <v>0.269422086520802</v>
       </c>
       <c r="H44" t="s">
         <v>9</v>
@@ -1669,22 +1813,22 @@
         <v>52</v>
       </c>
       <c r="B45" t="n">
-        <v>2.80101809243303</v>
+        <v>233.912785730475</v>
       </c>
       <c r="C45" t="n">
-        <v>-1.06369311352419</v>
+        <v>-1.33676439840693</v>
       </c>
       <c r="D45" t="n">
-        <v>0.050808138790976</v>
+        <v>0.512382196697274</v>
       </c>
       <c r="E45" t="n">
-        <v>-20.9354866924019</v>
+        <v>-2.60892046410565</v>
       </c>
       <c r="F45" t="n">
-        <v>0.000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000254453213527484</v>
+        <v>0.00908283506330976</v>
       </c>
       <c r="G45" t="n">
-        <v>0.0000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000187532018369755</v>
+        <v>0.271800079933937</v>
       </c>
       <c r="H45" t="s">
         <v>9</v>
@@ -1695,22 +1839,22 @@
         <v>53</v>
       </c>
       <c r="B46" t="n">
-        <v>5.51431564031539</v>
+        <v>545.566703815256</v>
       </c>
       <c r="C46" t="n">
-        <v>-1.09599291879357</v>
+        <v>-1.03212018056929</v>
       </c>
       <c r="D46" t="n">
-        <v>0.0536065433249264</v>
+        <v>0.400114658425701</v>
       </c>
       <c r="E46" t="n">
-        <v>-20.4451332023108</v>
+        <v>-2.57956103040635</v>
       </c>
       <c r="F46" t="n">
-        <v>0.00000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000663768603544681</v>
+        <v>0.00989259764539132</v>
       </c>
       <c r="G46" t="n">
-        <v>0.000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000423343956472295</v>
+        <v>0.291017682631512</v>
       </c>
       <c r="H46" t="s">
         <v>9</v>
@@ -1721,22 +1865,22 @@
         <v>54</v>
       </c>
       <c r="B47" t="n">
-        <v>10.1059472556159</v>
+        <v>99.7135176866414</v>
       </c>
       <c r="C47" t="n">
-        <v>-1.00044505441699</v>
+        <v>-10.0751920229102</v>
       </c>
       <c r="D47" t="n">
-        <v>0.0513739769596292</v>
+        <v>3.98882999279225</v>
       </c>
       <c r="E47" t="n">
-        <v>-19.473770839333</v>
+        <v>-2.52585145045436</v>
       </c>
       <c r="F47" t="n">
-        <v>0.00000000000000000000000000000000000000000000000000000000000000000000000000000000000183270470440043</v>
+        <v>0.0115418273037841</v>
       </c>
       <c r="G47" t="n">
-        <v>0.000000000000000000000000000000000000000000000000000000000000000000000000000000000103019748341424</v>
+        <v>0.324474274040254</v>
       </c>
       <c r="H47" t="s">
         <v>9</v>
@@ -1747,22 +1891,22 @@
         <v>55</v>
       </c>
       <c r="B48" t="n">
-        <v>1.92399641155317</v>
+        <v>182.946517631177</v>
       </c>
       <c r="C48" t="n">
-        <v>-1.10642902698518</v>
+        <v>-1.40104099843002</v>
       </c>
       <c r="D48" t="n">
-        <v>0.05689241733672</v>
+        <v>0.557785106107463</v>
       </c>
       <c r="E48" t="n">
-        <v>-19.4477415230352</v>
+        <v>-2.51179349016196</v>
       </c>
       <c r="F48" t="n">
-        <v>0.00000000000000000000000000000000000000000000000000000000000000000000000000000000000304552588621246</v>
+        <v>0.0120119357571017</v>
       </c>
       <c r="G48" t="n">
-        <v>0.000000000000000000000000000000000000000000000000000000000000000000000000000000000169756077338212</v>
+        <v>0.336334201198848</v>
       </c>
       <c r="H48" t="s">
         <v>9</v>
@@ -1773,22 +1917,22 @@
         <v>56</v>
       </c>
       <c r="B49" t="n">
-        <v>15.1068539212628</v>
+        <v>333.303257239617</v>
       </c>
       <c r="C49" t="n">
-        <v>-1.40620481986648</v>
+        <v>-1.13577007826844</v>
       </c>
       <c r="D49" t="n">
-        <v>0.0741842241457103</v>
+        <v>0.457268736566139</v>
       </c>
       <c r="E49" t="n">
-        <v>-18.9555776320375</v>
+        <v>-2.48381310036088</v>
       </c>
       <c r="F49" t="n">
-        <v>0.000000000000000000000000000000000000000000000000000000000000000000000000000000039716920139323</v>
+        <v>0.0129984009728165</v>
       </c>
       <c r="G49" t="n">
-        <v>0.00000000000000000000000000000000000000000000000000000000000000000000000000000205814321315726</v>
+        <v>0.354003326494049</v>
       </c>
       <c r="H49" t="s">
         <v>9</v>
@@ -1799,22 +1943,22 @@
         <v>57</v>
       </c>
       <c r="B50" t="n">
-        <v>1.6859154124794</v>
+        <v>60.0457287304068</v>
       </c>
       <c r="C50" t="n">
-        <v>-1.02967906343525</v>
+        <v>-5.29381243570014</v>
       </c>
       <c r="D50" t="n">
-        <v>0.0543511527028986</v>
+        <v>2.13357756805293</v>
       </c>
       <c r="E50" t="n">
-        <v>-18.9449351527799</v>
+        <v>-2.48119052007619</v>
       </c>
       <c r="F50" t="n">
-        <v>0.000000000000000000000000000000000000000000000000000000000000000000000000000000048618957323687</v>
+        <v>0.0130944363332645</v>
       </c>
       <c r="G50" t="n">
-        <v>0.00000000000000000000000000000000000000000000000000000000000000000000000000000249991894517842</v>
+        <v>0.35523116776467</v>
       </c>
       <c r="H50" t="s">
         <v>9</v>
@@ -1825,24 +1969,1272 @@
         <v>58</v>
       </c>
       <c r="B51" t="n">
-        <v>10.2132811049804</v>
+        <v>327.64840686709</v>
       </c>
       <c r="C51" t="n">
-        <v>-1.0220495800639</v>
+        <v>-1.15561895814945</v>
       </c>
       <c r="D51" t="n">
-        <v>0.0543308138910054</v>
+        <v>0.471542614853233</v>
       </c>
       <c r="E51" t="n">
-        <v>-18.8116007633212</v>
+        <v>-2.45072008711056</v>
       </c>
       <c r="F51" t="n">
-        <v>0.00000000000000000000000000000000000000000000000000000000000000000000000000000060677596899056</v>
+        <v>0.0142570774129089</v>
       </c>
       <c r="G51" t="n">
-        <v>0.0000000000000000000000000000000000000000000000000000000000000000000000000000298129259430695</v>
+        <v>0.377948074991638</v>
       </c>
       <c r="H51" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" t="s">
+        <v>59</v>
+      </c>
+      <c r="B52" t="n">
+        <v>323.633671043773</v>
+      </c>
+      <c r="C52" t="n">
+        <v>-1.22361028466855</v>
+      </c>
+      <c r="D52" t="n">
+        <v>0.501127622940442</v>
+      </c>
+      <c r="E52" t="n">
+        <v>-2.44171390411254</v>
+      </c>
+      <c r="F52" t="n">
+        <v>0.0146177257386781</v>
+      </c>
+      <c r="G52" t="n">
+        <v>0.383138285150615</v>
+      </c>
+      <c r="H52" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" t="s">
+        <v>60</v>
+      </c>
+      <c r="B53" t="n">
+        <v>529.908122178659</v>
+      </c>
+      <c r="C53" t="n">
+        <v>-1.11229237378346</v>
+      </c>
+      <c r="D53" t="n">
+        <v>0.45845754683349</v>
+      </c>
+      <c r="E53" t="n">
+        <v>-2.42616220730998</v>
+      </c>
+      <c r="F53" t="n">
+        <v>0.0152594483037525</v>
+      </c>
+      <c r="G53" t="n">
+        <v>0.394032865088008</v>
+      </c>
+      <c r="H53" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" t="s">
+        <v>61</v>
+      </c>
+      <c r="B54" t="n">
+        <v>38.6813834162462</v>
+      </c>
+      <c r="C54" t="n">
+        <v>-3.3826153962595</v>
+      </c>
+      <c r="D54" t="n">
+        <v>1.4026073787127</v>
+      </c>
+      <c r="E54" t="n">
+        <v>-2.41166234229</v>
+      </c>
+      <c r="F54" t="n">
+        <v>0.0158799804848668</v>
+      </c>
+      <c r="G54" t="n">
+        <v>0.404548082691933</v>
+      </c>
+      <c r="H54" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" t="s">
+        <v>62</v>
+      </c>
+      <c r="B55" t="n">
+        <v>19.8572872181421</v>
+      </c>
+      <c r="C55" t="n">
+        <v>-7.73916936467428</v>
+      </c>
+      <c r="D55" t="n">
+        <v>3.21555307110512</v>
+      </c>
+      <c r="E55" t="n">
+        <v>-2.40679260877958</v>
+      </c>
+      <c r="F55" t="n">
+        <v>0.0160933060287603</v>
+      </c>
+      <c r="G55" t="n">
+        <v>0.40653090446564</v>
+      </c>
+      <c r="H55" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" t="s">
+        <v>63</v>
+      </c>
+      <c r="B56" t="n">
+        <v>19.8572872181421</v>
+      </c>
+      <c r="C56" t="n">
+        <v>-7.73916936467428</v>
+      </c>
+      <c r="D56" t="n">
+        <v>3.21555307110512</v>
+      </c>
+      <c r="E56" t="n">
+        <v>-2.40679260877958</v>
+      </c>
+      <c r="F56" t="n">
+        <v>0.0160933060287603</v>
+      </c>
+      <c r="G56" t="n">
+        <v>0.40653090446564</v>
+      </c>
+      <c r="H56" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" t="s">
+        <v>64</v>
+      </c>
+      <c r="B57" t="n">
+        <v>498.387558038841</v>
+      </c>
+      <c r="C57" t="n">
+        <v>-1.13342101583121</v>
+      </c>
+      <c r="D57" t="n">
+        <v>0.471765041022298</v>
+      </c>
+      <c r="E57" t="n">
+        <v>-2.40251166846769</v>
+      </c>
+      <c r="F57" t="n">
+        <v>0.016282915076486</v>
+      </c>
+      <c r="G57" t="n">
+        <v>0.409835681997331</v>
+      </c>
+      <c r="H57" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" t="s">
+        <v>65</v>
+      </c>
+      <c r="B58" t="n">
+        <v>37.5697681186306</v>
+      </c>
+      <c r="C58" t="n">
+        <v>-6.20923061223894</v>
+      </c>
+      <c r="D58" t="n">
+        <v>2.5915339636938</v>
+      </c>
+      <c r="E58" t="n">
+        <v>-2.395967291661</v>
+      </c>
+      <c r="F58" t="n">
+        <v>0.0165765694721628</v>
+      </c>
+      <c r="G58" t="n">
+        <v>0.415726051654385</v>
+      </c>
+      <c r="H58" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" t="s">
+        <v>66</v>
+      </c>
+      <c r="B59" t="n">
+        <v>282.922665987701</v>
+      </c>
+      <c r="C59" t="n">
+        <v>-1.15924729761938</v>
+      </c>
+      <c r="D59" t="n">
+        <v>0.485000906447464</v>
+      </c>
+      <c r="E59" t="n">
+        <v>-2.39019614645804</v>
+      </c>
+      <c r="F59" t="n">
+        <v>0.01683937674619</v>
+      </c>
+      <c r="G59" t="n">
+        <v>0.417575250334494</v>
+      </c>
+      <c r="H59" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60" t="s">
+        <v>67</v>
+      </c>
+      <c r="B60" t="n">
+        <v>171.401245894553</v>
+      </c>
+      <c r="C60" t="n">
+        <v>-1.36495420861922</v>
+      </c>
+      <c r="D60" t="n">
+        <v>0.571222548991883</v>
+      </c>
+      <c r="E60" t="n">
+        <v>-2.38953138497096</v>
+      </c>
+      <c r="F60" t="n">
+        <v>0.0168698824182357</v>
+      </c>
+      <c r="G60" t="n">
+        <v>0.417575250334494</v>
+      </c>
+      <c r="H60" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61" t="s">
+        <v>68</v>
+      </c>
+      <c r="B61" t="n">
+        <v>339.156463443741</v>
+      </c>
+      <c r="C61" t="n">
+        <v>-1.07629125252559</v>
+      </c>
+      <c r="D61" t="n">
+        <v>0.454549582439972</v>
+      </c>
+      <c r="E61" t="n">
+        <v>-2.36781925251846</v>
+      </c>
+      <c r="F61" t="n">
+        <v>0.0178932750389536</v>
+      </c>
+      <c r="G61" t="n">
+        <v>0.430794512614228</v>
+      </c>
+      <c r="H61" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="62">
+      <c r="A62" t="s">
+        <v>69</v>
+      </c>
+      <c r="B62" t="n">
+        <v>1137.10543384925</v>
+      </c>
+      <c r="C62" t="n">
+        <v>-1.18517424965596</v>
+      </c>
+      <c r="D62" t="n">
+        <v>0.501668754028541</v>
+      </c>
+      <c r="E62" t="n">
+        <v>-2.36246375748675</v>
+      </c>
+      <c r="F62" t="n">
+        <v>0.0181539164059113</v>
+      </c>
+      <c r="G62" t="n">
+        <v>0.432047855487225</v>
+      </c>
+      <c r="H62" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="63">
+      <c r="A63" t="s">
+        <v>70</v>
+      </c>
+      <c r="B63" t="n">
+        <v>321.43041057495</v>
+      </c>
+      <c r="C63" t="n">
+        <v>-1.28165577056727</v>
+      </c>
+      <c r="D63" t="n">
+        <v>0.542189795972928</v>
+      </c>
+      <c r="E63" t="n">
+        <v>-2.36385077713868</v>
+      </c>
+      <c r="F63" t="n">
+        <v>0.0180860958408332</v>
+      </c>
+      <c r="G63" t="n">
+        <v>0.432047855487225</v>
+      </c>
+      <c r="H63" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="64">
+      <c r="A64" t="s">
+        <v>71</v>
+      </c>
+      <c r="B64" t="n">
+        <v>24.7402360331302</v>
+      </c>
+      <c r="C64" t="n">
+        <v>-4.58051981244278</v>
+      </c>
+      <c r="D64" t="n">
+        <v>1.94358883991484</v>
+      </c>
+      <c r="E64" t="n">
+        <v>-2.35673292538739</v>
+      </c>
+      <c r="F64" t="n">
+        <v>0.0184365012246061</v>
+      </c>
+      <c r="G64" t="n">
+        <v>0.434254346412006</v>
+      </c>
+      <c r="H64" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="65">
+      <c r="A65" t="s">
+        <v>72</v>
+      </c>
+      <c r="B65" t="n">
+        <v>410.586395581745</v>
+      </c>
+      <c r="C65" t="n">
+        <v>-1.00517255510342</v>
+      </c>
+      <c r="D65" t="n">
+        <v>0.432279198633618</v>
+      </c>
+      <c r="E65" t="n">
+        <v>-2.32528550594303</v>
+      </c>
+      <c r="F65" t="n">
+        <v>0.0200566987954843</v>
+      </c>
+      <c r="G65" t="n">
+        <v>0.451081625813279</v>
+      </c>
+      <c r="H65" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="66">
+      <c r="A66" t="s">
+        <v>73</v>
+      </c>
+      <c r="B66" t="n">
+        <v>612.67074074921</v>
+      </c>
+      <c r="C66" t="n">
+        <v>-1.05057745696538</v>
+      </c>
+      <c r="D66" t="n">
+        <v>0.452980126791557</v>
+      </c>
+      <c r="E66" t="n">
+        <v>-2.31925728046082</v>
+      </c>
+      <c r="F66" t="n">
+        <v>0.0203810902734992</v>
+      </c>
+      <c r="G66" t="n">
+        <v>0.453983902194365</v>
+      </c>
+      <c r="H66" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="67">
+      <c r="A67" t="s">
+        <v>74</v>
+      </c>
+      <c r="B67" t="n">
+        <v>255.775707432619</v>
+      </c>
+      <c r="C67" t="n">
+        <v>-1.17035356485393</v>
+      </c>
+      <c r="D67" t="n">
+        <v>0.508434794052227</v>
+      </c>
+      <c r="E67" t="n">
+        <v>-2.30187543918112</v>
+      </c>
+      <c r="F67" t="n">
+        <v>0.0213421976613385</v>
+      </c>
+      <c r="G67" t="n">
+        <v>0.472373974904293</v>
+      </c>
+      <c r="H67" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="68">
+      <c r="A68" t="s">
+        <v>75</v>
+      </c>
+      <c r="B68" t="n">
+        <v>319.850661164686</v>
+      </c>
+      <c r="C68" t="n">
+        <v>-1.06925817776694</v>
+      </c>
+      <c r="D68" t="n">
+        <v>0.466926307401163</v>
+      </c>
+      <c r="E68" t="n">
+        <v>-2.28999343326416</v>
+      </c>
+      <c r="F68" t="n">
+        <v>0.0220216973209045</v>
+      </c>
+      <c r="G68" t="n">
+        <v>0.481301798499518</v>
+      </c>
+      <c r="H68" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="69">
+      <c r="A69" t="s">
+        <v>76</v>
+      </c>
+      <c r="B69" t="n">
+        <v>166.472608482227</v>
+      </c>
+      <c r="C69" t="n">
+        <v>-1.34377642301531</v>
+      </c>
+      <c r="D69" t="n">
+        <v>0.587832651906148</v>
+      </c>
+      <c r="E69" t="n">
+        <v>-2.28598465678605</v>
+      </c>
+      <c r="F69" t="n">
+        <v>0.0222551561881079</v>
+      </c>
+      <c r="G69" t="n">
+        <v>0.483373672721146</v>
+      </c>
+      <c r="H69" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="70">
+      <c r="A70" t="s">
+        <v>77</v>
+      </c>
+      <c r="B70" t="n">
+        <v>27.7955690333663</v>
+      </c>
+      <c r="C70" t="n">
+        <v>-5.76847136650035</v>
+      </c>
+      <c r="D70" t="n">
+        <v>2.53101240036769</v>
+      </c>
+      <c r="E70" t="n">
+        <v>-2.27911620095672</v>
+      </c>
+      <c r="F70" t="n">
+        <v>0.0226601587053347</v>
+      </c>
+      <c r="G70" t="n">
+        <v>0.486112696903364</v>
+      </c>
+      <c r="H70" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="71">
+      <c r="A71" t="s">
+        <v>78</v>
+      </c>
+      <c r="B71" t="n">
+        <v>265.183832183889</v>
+      </c>
+      <c r="C71" t="n">
+        <v>-1.12364840459141</v>
+      </c>
+      <c r="D71" t="n">
+        <v>0.495183112435014</v>
+      </c>
+      <c r="E71" t="n">
+        <v>-2.26915736093257</v>
+      </c>
+      <c r="F71" t="n">
+        <v>0.0232587581798821</v>
+      </c>
+      <c r="G71" t="n">
+        <v>0.494390433018713</v>
+      </c>
+      <c r="H71" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="72">
+      <c r="A72" t="s">
+        <v>79</v>
+      </c>
+      <c r="B72" t="n">
+        <v>365.756049503531</v>
+      </c>
+      <c r="C72" t="n">
+        <v>-1.00226124261468</v>
+      </c>
+      <c r="D72" t="n">
+        <v>0.442677662426364</v>
+      </c>
+      <c r="E72" t="n">
+        <v>-2.26408813383801</v>
+      </c>
+      <c r="F72" t="n">
+        <v>0.0235686946607767</v>
+      </c>
+      <c r="G72" t="n">
+        <v>0.496437882703731</v>
+      </c>
+      <c r="H72" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="73">
+      <c r="A73" t="s">
+        <v>80</v>
+      </c>
+      <c r="B73" t="n">
+        <v>308.540677641984</v>
+      </c>
+      <c r="C73" t="n">
+        <v>-1.06646830409756</v>
+      </c>
+      <c r="D73" t="n">
+        <v>0.473013814504047</v>
+      </c>
+      <c r="E73" t="n">
+        <v>-2.25462401180766</v>
+      </c>
+      <c r="F73" t="n">
+        <v>0.0241569389585666</v>
+      </c>
+      <c r="G73" t="n">
+        <v>0.507295718129898</v>
+      </c>
+      <c r="H73" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="74">
+      <c r="A74" t="s">
+        <v>81</v>
+      </c>
+      <c r="B74" t="n">
+        <v>413.334559693384</v>
+      </c>
+      <c r="C74" t="n">
+        <v>-1.15104969070565</v>
+      </c>
+      <c r="D74" t="n">
+        <v>0.513169128030728</v>
+      </c>
+      <c r="E74" t="n">
+        <v>-2.24302209122122</v>
+      </c>
+      <c r="F74" t="n">
+        <v>0.0248953899774892</v>
+      </c>
+      <c r="G74" t="n">
+        <v>0.516066723031559</v>
+      </c>
+      <c r="H74" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="75">
+      <c r="A75" t="s">
+        <v>82</v>
+      </c>
+      <c r="B75" t="n">
+        <v>213.743876681281</v>
+      </c>
+      <c r="C75" t="n">
+        <v>-1.17926496018594</v>
+      </c>
+      <c r="D75" t="n">
+        <v>0.52664534937371</v>
+      </c>
+      <c r="E75" t="n">
+        <v>-2.23920131752485</v>
+      </c>
+      <c r="F75" t="n">
+        <v>0.0251428201665476</v>
+      </c>
+      <c r="G75" t="n">
+        <v>0.516066723031559</v>
+      </c>
+      <c r="H75" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="76">
+      <c r="A76" t="s">
+        <v>83</v>
+      </c>
+      <c r="B76" t="n">
+        <v>325.001924342077</v>
+      </c>
+      <c r="C76" t="n">
+        <v>-1.20737947135903</v>
+      </c>
+      <c r="D76" t="n">
+        <v>0.538848276058908</v>
+      </c>
+      <c r="E76" t="n">
+        <v>-2.24066685373794</v>
+      </c>
+      <c r="F76" t="n">
+        <v>0.0250476626941828</v>
+      </c>
+      <c r="G76" t="n">
+        <v>0.516066723031559</v>
+      </c>
+      <c r="H76" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="77">
+      <c r="A77" t="s">
+        <v>84</v>
+      </c>
+      <c r="B77" t="n">
+        <v>230.677772382588</v>
+      </c>
+      <c r="C77" t="n">
+        <v>-8.84219111568682</v>
+      </c>
+      <c r="D77" t="n">
+        <v>3.94476745024261</v>
+      </c>
+      <c r="E77" t="n">
+        <v>-2.24149870105601</v>
+      </c>
+      <c r="F77" t="n">
+        <v>0.0249937895733439</v>
+      </c>
+      <c r="G77" t="n">
+        <v>0.516066723031559</v>
+      </c>
+      <c r="H77" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="78">
+      <c r="A78" t="s">
+        <v>85</v>
+      </c>
+      <c r="B78" t="n">
+        <v>119.520801119194</v>
+      </c>
+      <c r="C78" t="n">
+        <v>-1.58945132267326</v>
+      </c>
+      <c r="D78" t="n">
+        <v>0.71087112078223</v>
+      </c>
+      <c r="E78" t="n">
+        <v>-2.23592051527463</v>
+      </c>
+      <c r="F78" t="n">
+        <v>0.0253569782129315</v>
+      </c>
+      <c r="G78" t="n">
+        <v>0.516926468130288</v>
+      </c>
+      <c r="H78" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="79">
+      <c r="A79" t="s">
+        <v>86</v>
+      </c>
+      <c r="B79" t="n">
+        <v>512.736245113923</v>
+      </c>
+      <c r="C79" t="n">
+        <v>-1.08973101727015</v>
+      </c>
+      <c r="D79" t="n">
+        <v>0.488183994330565</v>
+      </c>
+      <c r="E79" t="n">
+        <v>-2.23221373483265</v>
+      </c>
+      <c r="F79" t="n">
+        <v>0.0256008400799207</v>
+      </c>
+      <c r="G79" t="n">
+        <v>0.520376259583695</v>
+      </c>
+      <c r="H79" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="80">
+      <c r="A80" t="s">
+        <v>87</v>
+      </c>
+      <c r="B80" t="n">
+        <v>35.8263249259779</v>
+      </c>
+      <c r="C80" t="n">
+        <v>-3.77308393282856</v>
+      </c>
+      <c r="D80" t="n">
+        <v>1.71471433308851</v>
+      </c>
+      <c r="E80" t="n">
+        <v>-2.20041546280923</v>
+      </c>
+      <c r="F80" t="n">
+        <v>0.0277774317468829</v>
+      </c>
+      <c r="G80" t="n">
+        <v>0.551750011792785</v>
+      </c>
+      <c r="H80" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="81">
+      <c r="A81" t="s">
+        <v>88</v>
+      </c>
+      <c r="B81" t="n">
+        <v>906.30805114327</v>
+      </c>
+      <c r="C81" t="n">
+        <v>-1.02338621109136</v>
+      </c>
+      <c r="D81" t="n">
+        <v>0.470516216097527</v>
+      </c>
+      <c r="E81" t="n">
+        <v>-2.17502856666525</v>
+      </c>
+      <c r="F81" t="n">
+        <v>0.029627975743681</v>
+      </c>
+      <c r="G81" t="n">
+        <v>0.565934922972448</v>
+      </c>
+      <c r="H81" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="82">
+      <c r="A82" t="s">
+        <v>89</v>
+      </c>
+      <c r="B82" t="n">
+        <v>48.4626839691111</v>
+      </c>
+      <c r="C82" t="n">
+        <v>-4.56828148899534</v>
+      </c>
+      <c r="D82" t="n">
+        <v>2.09901504135066</v>
+      </c>
+      <c r="E82" t="n">
+        <v>-2.17639292668231</v>
+      </c>
+      <c r="F82" t="n">
+        <v>0.0295258922487638</v>
+      </c>
+      <c r="G82" t="n">
+        <v>0.565934922972448</v>
+      </c>
+      <c r="H82" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="83">
+      <c r="A83" t="s">
+        <v>90</v>
+      </c>
+      <c r="B83" t="n">
+        <v>321.489216380867</v>
+      </c>
+      <c r="C83" t="n">
+        <v>-1.08189590434783</v>
+      </c>
+      <c r="D83" t="n">
+        <v>0.500500967353209</v>
+      </c>
+      <c r="E83" t="n">
+        <v>-2.16162600058338</v>
+      </c>
+      <c r="F83" t="n">
+        <v>0.0306470156694566</v>
+      </c>
+      <c r="G83" t="n">
+        <v>0.571382751398062</v>
+      </c>
+      <c r="H83" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="84">
+      <c r="A84" t="s">
+        <v>91</v>
+      </c>
+      <c r="B84" t="n">
+        <v>23.0937387070035</v>
+      </c>
+      <c r="C84" t="n">
+        <v>-4.47895226247242</v>
+      </c>
+      <c r="D84" t="n">
+        <v>2.06911124862084</v>
+      </c>
+      <c r="E84" t="n">
+        <v>-2.16467445404778</v>
+      </c>
+      <c r="F84" t="n">
+        <v>0.0304126247542808</v>
+      </c>
+      <c r="G84" t="n">
+        <v>0.571382751398062</v>
+      </c>
+      <c r="H84" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="85">
+      <c r="A85" t="s">
+        <v>92</v>
+      </c>
+      <c r="B85" t="n">
+        <v>57.3743418395301</v>
+      </c>
+      <c r="C85" t="n">
+        <v>-4.20735544655822</v>
+      </c>
+      <c r="D85" t="n">
+        <v>1.98047672390171</v>
+      </c>
+      <c r="E85" t="n">
+        <v>-2.12441549844088</v>
+      </c>
+      <c r="F85" t="n">
+        <v>0.0336354151575159</v>
+      </c>
+      <c r="G85" t="n">
+        <v>0.600219524368473</v>
+      </c>
+      <c r="H85" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="86">
+      <c r="A86" t="s">
+        <v>93</v>
+      </c>
+      <c r="B86" t="n">
+        <v>312.749114369592</v>
+      </c>
+      <c r="C86" t="n">
+        <v>-1.33061854674322</v>
+      </c>
+      <c r="D86" t="n">
+        <v>0.632026380234124</v>
+      </c>
+      <c r="E86" t="n">
+        <v>-2.10532121499473</v>
+      </c>
+      <c r="F86" t="n">
+        <v>0.0352633566216262</v>
+      </c>
+      <c r="G86" t="n">
+        <v>0.613107537072264</v>
+      </c>
+      <c r="H86" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="87">
+      <c r="A87" t="s">
+        <v>94</v>
+      </c>
+      <c r="B87" t="n">
+        <v>294.625531507445</v>
+      </c>
+      <c r="C87" t="n">
+        <v>-1.08879367772939</v>
+      </c>
+      <c r="D87" t="n">
+        <v>0.522952824369598</v>
+      </c>
+      <c r="E87" t="n">
+        <v>-2.08201127710114</v>
+      </c>
+      <c r="F87" t="n">
+        <v>0.03734143967047</v>
+      </c>
+      <c r="G87" t="n">
+        <v>0.634986627762236</v>
+      </c>
+      <c r="H87" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="88">
+      <c r="A88" t="s">
+        <v>95</v>
+      </c>
+      <c r="B88" t="n">
+        <v>722.705175977724</v>
+      </c>
+      <c r="C88" t="n">
+        <v>-1.0096671145296</v>
+      </c>
+      <c r="D88" t="n">
+        <v>0.492278198532486</v>
+      </c>
+      <c r="E88" t="n">
+        <v>-2.05100920077202</v>
+      </c>
+      <c r="F88" t="n">
+        <v>0.0402660507449409</v>
+      </c>
+      <c r="G88" t="n">
+        <v>0.661996557772928</v>
+      </c>
+      <c r="H88" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="89">
+      <c r="A89" t="s">
+        <v>96</v>
+      </c>
+      <c r="B89" t="n">
+        <v>27.5175046782152</v>
+      </c>
+      <c r="C89" t="n">
+        <v>-4.74029575300924</v>
+      </c>
+      <c r="D89" t="n">
+        <v>2.31275522619237</v>
+      </c>
+      <c r="E89" t="n">
+        <v>-2.04963140903305</v>
+      </c>
+      <c r="F89" t="n">
+        <v>0.0404004129977734</v>
+      </c>
+      <c r="G89" t="n">
+        <v>0.661996557772928</v>
+      </c>
+      <c r="H89" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="90">
+      <c r="A90" t="s">
+        <v>97</v>
+      </c>
+      <c r="B90" t="n">
+        <v>533.343588101152</v>
+      </c>
+      <c r="C90" t="n">
+        <v>-7.72712897142133</v>
+      </c>
+      <c r="D90" t="n">
+        <v>3.77395026283281</v>
+      </c>
+      <c r="E90" t="n">
+        <v>-2.04749094006903</v>
+      </c>
+      <c r="F90" t="n">
+        <v>0.040609905519042</v>
+      </c>
+      <c r="G90" t="n">
+        <v>0.661996557772928</v>
+      </c>
+      <c r="H90" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="91">
+      <c r="A91" t="s">
+        <v>98</v>
+      </c>
+      <c r="B91" t="n">
+        <v>204.645095737349</v>
+      </c>
+      <c r="C91" t="n">
+        <v>-1.09018736940807</v>
+      </c>
+      <c r="D91" t="n">
+        <v>0.533848841656982</v>
+      </c>
+      <c r="E91" t="n">
+        <v>-2.04212744196335</v>
+      </c>
+      <c r="F91" t="n">
+        <v>0.0411388914412914</v>
+      </c>
+      <c r="G91" t="n">
+        <v>0.665476452734765</v>
+      </c>
+      <c r="H91" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="92">
+      <c r="A92" t="s">
+        <v>99</v>
+      </c>
+      <c r="B92" t="n">
+        <v>17.4614115716502</v>
+      </c>
+      <c r="C92" t="n">
+        <v>-7.55592133110542</v>
+      </c>
+      <c r="D92" t="n">
+        <v>3.72891760309568</v>
+      </c>
+      <c r="E92" t="n">
+        <v>-2.02630418136154</v>
+      </c>
+      <c r="F92" t="n">
+        <v>0.042733623042272</v>
+      </c>
+      <c r="G92" t="n">
+        <v>0.678676127222597</v>
+      </c>
+      <c r="H92" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="93">
+      <c r="A93" t="s">
+        <v>100</v>
+      </c>
+      <c r="B93" t="n">
+        <v>65.2923630601048</v>
+      </c>
+      <c r="C93" t="n">
+        <v>-1.8919061021691</v>
+      </c>
+      <c r="D93" t="n">
+        <v>0.936214557634542</v>
+      </c>
+      <c r="E93" t="n">
+        <v>-2.02080397782878</v>
+      </c>
+      <c r="F93" t="n">
+        <v>0.0433000608937399</v>
+      </c>
+      <c r="G93" t="n">
+        <v>0.682330492210329</v>
+      </c>
+      <c r="H93" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="94">
+      <c r="A94" t="s">
+        <v>101</v>
+      </c>
+      <c r="B94" t="n">
+        <v>200.894374469373</v>
+      </c>
+      <c r="C94" t="n">
+        <v>-1.09346747123286</v>
+      </c>
+      <c r="D94" t="n">
+        <v>0.542139513608468</v>
+      </c>
+      <c r="E94" t="n">
+        <v>-2.01694848610972</v>
+      </c>
+      <c r="F94" t="n">
+        <v>0.0437008894373723</v>
+      </c>
+      <c r="G94" t="n">
+        <v>0.684680002600808</v>
+      </c>
+      <c r="H94" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="95">
+      <c r="A95" t="s">
+        <v>102</v>
+      </c>
+      <c r="B95" t="n">
+        <v>877.930462946595</v>
+      </c>
+      <c r="C95" t="n">
+        <v>-1.00434748803268</v>
+      </c>
+      <c r="D95" t="n">
+        <v>0.50608082902213</v>
+      </c>
+      <c r="E95" t="n">
+        <v>-1.98455944275408</v>
+      </c>
+      <c r="F95" t="n">
+        <v>0.0471935084334889</v>
+      </c>
+      <c r="G95" t="n">
+        <v>0.700070512336776</v>
+      </c>
+      <c r="H95" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="96">
+      <c r="A96" t="s">
+        <v>103</v>
+      </c>
+      <c r="B96" t="n">
+        <v>144.985182523862</v>
+      </c>
+      <c r="C96" t="n">
+        <v>-7.1678314826983</v>
+      </c>
+      <c r="D96" t="n">
+        <v>3.61455655779224</v>
+      </c>
+      <c r="E96" t="n">
+        <v>-1.98304587799185</v>
+      </c>
+      <c r="F96" t="n">
+        <v>0.0473623051866521</v>
+      </c>
+      <c r="G96" t="n">
+        <v>0.701082785055921</v>
+      </c>
+      <c r="H96" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="97">
+      <c r="A97" t="s">
+        <v>104</v>
+      </c>
+      <c r="B97" t="n">
+        <v>165.048266780253</v>
+      </c>
+      <c r="C97" t="n">
+        <v>-1.14928804751001</v>
+      </c>
+      <c r="D97" t="n">
+        <v>0.580334355754517</v>
+      </c>
+      <c r="E97" t="n">
+        <v>-1.98038947050752</v>
+      </c>
+      <c r="F97" t="n">
+        <v>0.0476597822002937</v>
+      </c>
+      <c r="G97" t="n">
+        <v>0.703991528602643</v>
+      </c>
+      <c r="H97" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="98">
+      <c r="A98" t="s">
+        <v>105</v>
+      </c>
+      <c r="B98" t="n">
+        <v>56.5684203557727</v>
+      </c>
+      <c r="C98" t="n">
+        <v>-3.75771936017139</v>
+      </c>
+      <c r="D98" t="n">
+        <v>1.90226688152342</v>
+      </c>
+      <c r="E98" t="n">
+        <v>-1.97539020243155</v>
+      </c>
+      <c r="F98" t="n">
+        <v>0.0482238837980459</v>
+      </c>
+      <c r="G98" t="n">
+        <v>0.706338062689026</v>
+      </c>
+      <c r="H98" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="99">
+      <c r="A99" t="s">
+        <v>106</v>
+      </c>
+      <c r="B99" t="n">
+        <v>82.5833233459182</v>
+      </c>
+      <c r="C99" t="n">
+        <v>-1.51267690401259</v>
+      </c>
+      <c r="D99" t="n">
+        <v>0.768414711244905</v>
+      </c>
+      <c r="E99" t="n">
+        <v>-1.96856838094876</v>
+      </c>
+      <c r="F99" t="n">
+        <v>0.0490026764824369</v>
+      </c>
+      <c r="G99" t="n">
+        <v>0.711155765655198</v>
+      </c>
+      <c r="H99" t="s">
         <v>9</v>
       </c>
     </row>

</xml_diff>